<commit_message>
AUTO FROM work 14.02.2024  8:48:36,02
</commit_message>
<xml_diff>
--- a/poluyanov/minvent/Win32/Debug/mater.xlsx
+++ b/poluyanov/minvent/Win32/Debug/mater.xlsx
@@ -15,9 +15,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Лица ответственные за оборудование/инструменты/материалы</t>
+  </si>
+  <si>
+    <t>срок годности</t>
+  </si>
+  <si>
+    <t>кол-во</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,6 +39,21 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,8 +76,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -58,6 +95,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -350,13 +390,1441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:O100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>